<commit_message>
DONE cảm ơn partner
</commit_message>
<xml_diff>
--- a/Team/Capstone-Diner.xlsx
+++ b/Team/Capstone-Diner.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="34">
   <si>
     <t>Header</t>
   </si>
@@ -130,6 +130,9 @@
   </si>
   <si>
     <t>BacktoTop</t>
+  </si>
+  <si>
+    <t>Deloy</t>
   </si>
 </sst>
 </file>
@@ -1395,10 +1398,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:G983"/>
+  <dimension ref="B1:G984"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.69921875" defaultRowHeight="15" customHeight="1" outlineLevelRow="2" x14ac:dyDescent="0.25"/>
@@ -1552,7 +1555,7 @@
         <v>18</v>
       </c>
       <c r="D12" s="8">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>31</v>
@@ -1565,7 +1568,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="34">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="E13" s="35" t="s">
         <v>31</v>
@@ -1586,7 +1589,7 @@
       <c r="E16" s="22"/>
       <c r="G16" s="1"/>
     </row>
-    <row r="17" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7" ht="19.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="54"/>
       <c r="C17" s="23" t="s">
         <v>20</v>
@@ -1600,40 +1603,46 @@
     <row r="18" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="54"/>
       <c r="C18" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E18" s="24"/>
       <c r="G18" s="1"/>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B19" s="55"/>
-      <c r="C19" s="25" t="s">
+    <row r="19" spans="2:7" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="54"/>
+      <c r="C19" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" s="19"/>
+      <c r="E19" s="24" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" s="1"/>
+    </row>
+    <row r="20" spans="2:7" ht="18.600000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="55"/>
+      <c r="C20" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D19" s="26"/>
-      <c r="E19" s="27" t="s">
+      <c r="D20" s="26"/>
+      <c r="E20" s="27" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="45" t="s">
+    <row r="21" spans="2:7" ht="27.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="28">
+      <c r="C21" s="46"/>
+      <c r="D21" s="28">
         <v>1</v>
       </c>
-      <c r="E20" s="29">
+      <c r="E21" s="29">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -1645,7 +1654,11 @@
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
     <row r="25" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2605,15 +2618,16 @@
     <row r="981" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="982" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="983" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="984" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="F3:G7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C3:C8"/>
-    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
     <mergeCell ref="F2:G2"/>
     <mergeCell ref="F8:G12"/>
-    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B16:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>